<commit_message>
#fix add event bug #edit footer
</commit_message>
<xml_diff>
--- a/SupplyChain.App/permissions.xlsx
+++ b/SupplyChain.App/permissions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>CanAddUser</t>
   </si>
@@ -43,6 +43,21 @@
   </si>
   <si>
     <t>HasAccessToProduct</t>
+  </si>
+  <si>
+    <t>CanAddEvent</t>
+  </si>
+  <si>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>202cb962ac59075b964b07152d234b70</t>
+  </si>
+  <si>
+    <t>egypt</t>
+  </si>
+  <si>
+    <t>a@mail.com</t>
   </si>
 </sst>
 </file>
@@ -364,43 +379,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1">
+        <v>1148177915</v>
+      </c>
+      <c r="J1" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -408,46 +450,51 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B9">
+  <sortState ref="A1:A9">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#edit Event #publish Event
</commit_message>
<xml_diff>
--- a/SupplyChain.App/permissions.xlsx
+++ b/SupplyChain.App/permissions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>CanAddUser</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>a@mail.com</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>HasPermissionToPublishEvent</t>
   </si>
 </sst>
 </file>
@@ -379,16 +385,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
@@ -433,6 +439,9 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -488,6 +497,14 @@
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>